<commit_message>
Session 12 update with new strategy added for last two sessions
</commit_message>
<xml_diff>
--- a/data/GASY_status_all.xlsx
+++ b/data/GASY_status_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GASY/participant_2_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124B2A9A-6357-C04A-B47C-8C502EFFB9EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45108978-E40C-7C4F-9E79-3533ADC9EE0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33660" yWindow="5440" windowWidth="28800" windowHeight="16160" xr2:uid="{3C916DE0-195B-2A4F-AB3E-F4618B8BB61D}"/>
   </bookViews>
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D24135B-7C4E-9B44-8B3B-A592D6651794}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,6 +494,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Session 13 updates - all data collected
</commit_message>
<xml_diff>
--- a/data/GASY_status_all.xlsx
+++ b/data/GASY_status_all.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GASY/participant_2_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45108978-E40C-7C4F-9E79-3533ADC9EE0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDD0E62-1560-6B49-8356-E5FCEBA54A33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33660" yWindow="5440" windowWidth="28800" windowHeight="16160" xr2:uid="{3C916DE0-195B-2A4F-AB3E-F4618B8BB61D}"/>
   </bookViews>
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D24135B-7C4E-9B44-8B3B-A592D6651794}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,6 +502,14 @@
         <v>60</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>